<commit_message>
Update question de con bio
</commit_message>
<xml_diff>
--- a/Excel/Secret.xlsx
+++ b/Excel/Secret.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moito\Desktop\Sérieux\Projet\Site web\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0C4711-766A-4E3C-9D1C-C3196517292C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAB3D22-A53C-4FAF-93F6-5D00608C9EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="60" windowWidth="21600" windowHeight="11385" xr2:uid="{0C1EC4D3-5916-499C-9244-5ABC4AEA4E79}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{0C1EC4D3-5916-499C-9244-5ABC4AEA4E79}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1540,8 +1540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4434D7D-6CBE-4AEC-87F6-B0BB4C058CB9}">
   <dimension ref="A1:F151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,7 +3242,7 @@
         <v>199</v>
       </c>
       <c r="D85" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85" t="s">
         <v>198</v>

</xml_diff>